<commit_message>
Added more mouser sources including transistors and switches.
</commit_message>
<xml_diff>
--- a/ChaprSVN/PriceSourceList v1.xlsx
+++ b/ChaprSVN/PriceSourceList v1.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="72">
   <si>
     <t>Part Name</t>
   </si>
@@ -135,9 +135,6 @@
     <t>- costs for transistors/resistors/diodes are based upon purchase of 100</t>
   </si>
   <si>
-    <t>2N3405 transistor</t>
-  </si>
-  <si>
     <t>Case - Serpac 9v holder</t>
   </si>
   <si>
@@ -210,9 +207,6 @@
     <t>9V battery - lithium 1200mAh</t>
   </si>
   <si>
-    <t>2N3403 (3904) transistor</t>
-  </si>
-  <si>
     <t>(opt) arduino programmer</t>
   </si>
   <si>
@@ -241,6 +235,36 @@
   </si>
   <si>
     <t>SRA21B-ND</t>
+  </si>
+  <si>
+    <t>- same exact switch - RS is cheaper for singles</t>
+  </si>
+  <si>
+    <t>112-R13-24A-B(R)(W)</t>
+  </si>
+  <si>
+    <t>- current estimate</t>
+  </si>
+  <si>
+    <t>- wrong part number!  Need the diffused blue version (more expensive)</t>
+  </si>
+  <si>
+    <t>2N3904 transistor</t>
+  </si>
+  <si>
+    <t>2N3906 transistor</t>
+  </si>
+  <si>
+    <t>512-2N3904BU</t>
+  </si>
+  <si>
+    <t>- TO-92 EBC - at 100 quantity, $0.056, bulk</t>
+  </si>
+  <si>
+    <t>512-2N3906BU</t>
+  </si>
+  <si>
+    <t>- TO-92 EBC - at 100 quantity, $0.057, bulk</t>
   </si>
 </sst>
 </file>
@@ -252,7 +276,7 @@
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -276,20 +300,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="12"/>
-      <color theme="1"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <i/>
       <sz val="9"/>
       <color theme="1"/>
@@ -304,17 +314,46 @@
       <family val="2"/>
     </font>
     <font>
+      <b/>
       <i/>
-      <sz val="12"/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
     <font>
-      <b/>
-      <i/>
-      <sz val="11"/>
+      <sz val="10"/>
       <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -361,13 +400,11 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="3"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -382,7 +419,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="8" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -390,14 +427,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="3" applyFont="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -705,7 +746,7 @@
   <dimension ref="B3:K32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A32" sqref="A32:XFD32"/>
+      <selection activeCell="K22" sqref="K22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -720,542 +761,567 @@
   </cols>
   <sheetData>
     <row r="3" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B3" s="19" t="s">
+      <c r="B3" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="20" t="s">
+      <c r="C3" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="20" t="s">
-        <v>1</v>
-      </c>
-      <c r="E3" s="21" t="s">
+      <c r="D3" s="17" t="s">
+        <v>1</v>
+      </c>
+      <c r="E3" s="18" t="s">
         <v>14</v>
       </c>
-      <c r="F3" s="19" t="s">
+      <c r="F3" s="16" t="s">
         <v>10</v>
       </c>
-      <c r="G3" s="19" t="s">
+      <c r="G3" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="H3" s="19" t="s">
+      <c r="H3" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="I3" s="19" t="s">
+      <c r="I3" s="16" t="s">
         <v>12</v>
       </c>
-      <c r="J3" s="19" t="s">
+      <c r="J3" s="16" t="s">
         <v>18</v>
       </c>
-      <c r="K3" s="20" t="s">
-        <v>34</v>
+      <c r="K3" s="17" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="4" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B4" s="7">
+      <c r="B4" s="5">
         <v>1</v>
       </c>
       <c r="C4" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="9">
+      <c r="D4" s="7">
         <v>27.05</v>
       </c>
       <c r="E4" s="1">
         <f>D4*B4</f>
         <v>27.05</v>
       </c>
-      <c r="F4" s="16" t="s">
+      <c r="F4" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="G4" s="14"/>
+      <c r="H4" s="14"/>
+      <c r="I4" s="14"/>
+      <c r="J4" s="14" t="s">
         <v>36</v>
       </c>
-      <c r="G4" s="16"/>
-      <c r="H4" s="16"/>
-      <c r="I4" s="16"/>
-      <c r="J4" s="16" t="s">
-        <v>37</v>
-      </c>
       <c r="K4" s="2"/>
     </row>
-    <row r="5" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B5" s="7">
-        <v>1</v>
-      </c>
-      <c r="C5" s="15" t="s">
+    <row r="5" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B5" s="5">
+        <v>1</v>
+      </c>
+      <c r="C5" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="D5" s="8">
+      <c r="D5" s="6">
         <v>15.95</v>
       </c>
       <c r="E5" s="1">
         <f t="shared" ref="E5:E23" si="0">D5*B5</f>
         <v>15.95</v>
       </c>
-      <c r="F5" s="6" t="s">
+      <c r="F5" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="G5" s="4"/>
+      <c r="H5" s="4"/>
+      <c r="I5" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="J5" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="G5" s="6"/>
-      <c r="H5" s="6"/>
-      <c r="I5" s="6" t="s">
-        <v>31</v>
-      </c>
-      <c r="J5" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="K5" s="18" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="6" spans="2:11" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B6" s="7">
+      <c r="K5" s="20" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="6" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B6" s="5">
         <v>1</v>
       </c>
       <c r="C6" t="s">
-        <v>60</v>
-      </c>
-      <c r="D6" s="8">
+        <v>58</v>
+      </c>
+      <c r="D6" s="6">
         <v>8.9600000000000009</v>
       </c>
       <c r="E6" s="1">
         <f t="shared" si="0"/>
         <v>8.9600000000000009</v>
       </c>
-      <c r="F6" s="6"/>
-      <c r="G6" s="6"/>
-      <c r="H6" s="6"/>
-      <c r="I6" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="J6" s="6"/>
-      <c r="K6" s="3"/>
+      <c r="F6" s="4"/>
+      <c r="G6" s="4"/>
+      <c r="H6" s="4"/>
+      <c r="I6" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="J6" s="4"/>
+      <c r="K6" s="21"/>
     </row>
     <row r="7" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B7" s="7">
+      <c r="B7" s="5">
         <v>1</v>
       </c>
       <c r="C7" t="s">
         <v>15</v>
       </c>
-      <c r="D7" s="8">
+      <c r="D7" s="6">
         <v>0.09</v>
       </c>
       <c r="E7" s="1">
         <f t="shared" si="0"/>
         <v>0.09</v>
       </c>
-      <c r="F7" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="G7" s="6"/>
-      <c r="H7" s="6"/>
-      <c r="I7" s="6"/>
-      <c r="J7" s="6"/>
+      <c r="F7" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="G7" s="4"/>
+      <c r="H7" s="4"/>
+      <c r="I7" s="4"/>
+      <c r="J7" s="4"/>
+      <c r="K7" s="22"/>
     </row>
     <row r="8" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B8" s="7">
+      <c r="B8" s="5">
         <v>1</v>
       </c>
       <c r="C8" t="s">
         <v>16</v>
       </c>
-      <c r="D8" s="8">
+      <c r="D8" s="6">
         <v>0.23</v>
       </c>
       <c r="E8" s="1">
         <f t="shared" si="0"/>
         <v>0.23</v>
       </c>
-      <c r="F8" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="G8" s="6"/>
-      <c r="H8" s="6"/>
-      <c r="I8" s="6"/>
-      <c r="J8" s="6"/>
+      <c r="F8" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="G8" s="4"/>
+      <c r="H8" s="4"/>
+      <c r="I8" s="4"/>
+      <c r="J8" s="4"/>
+      <c r="K8" s="19" t="s">
+        <v>65</v>
+      </c>
     </row>
     <row r="9" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B9" s="7">
+      <c r="B9" s="5">
         <v>1</v>
       </c>
       <c r="C9" t="s">
         <v>6</v>
       </c>
-      <c r="D9" s="8">
+      <c r="D9" s="6">
         <v>0.3</v>
       </c>
       <c r="E9" s="1">
         <f t="shared" si="0"/>
         <v>0.3</v>
       </c>
-      <c r="F9" s="6"/>
-      <c r="G9" s="6"/>
-      <c r="H9" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="I9" s="6"/>
-      <c r="J9" s="6"/>
+      <c r="F9" s="4"/>
+      <c r="G9" s="4"/>
+      <c r="H9" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="I9" s="4"/>
+      <c r="J9" s="4"/>
+      <c r="K9" s="22"/>
     </row>
     <row r="10" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B10" s="7">
+      <c r="B10" s="5">
         <v>1</v>
       </c>
       <c r="C10" t="s">
-        <v>52</v>
-      </c>
-      <c r="D10" s="8">
+        <v>51</v>
+      </c>
+      <c r="D10" s="6">
         <v>6.77</v>
       </c>
       <c r="E10" s="1">
         <f t="shared" si="0"/>
         <v>6.77</v>
       </c>
-      <c r="F10" s="6" t="s">
+      <c r="F10" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="G10" s="4"/>
+      <c r="H10" s="4"/>
+      <c r="I10" s="4"/>
+      <c r="J10" s="4"/>
+      <c r="K10" s="19" t="s">
         <v>47</v>
       </c>
-      <c r="G10" s="6"/>
-      <c r="H10" s="6"/>
-      <c r="I10" s="6"/>
-      <c r="J10" s="6"/>
-      <c r="K10" s="4" t="s">
-        <v>48</v>
-      </c>
     </row>
     <row r="11" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B11" s="7">
+      <c r="B11" s="5">
         <v>1</v>
       </c>
       <c r="C11" t="s">
         <v>20</v>
       </c>
-      <c r="D11" s="8">
+      <c r="D11" s="6">
         <v>0.44</v>
       </c>
       <c r="E11" s="1">
         <f t="shared" si="0"/>
         <v>0.44</v>
       </c>
-      <c r="F11" s="6" t="s">
+      <c r="F11" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="G11" s="4"/>
+      <c r="H11" s="4"/>
+      <c r="I11" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="J11" s="4"/>
+      <c r="K11" s="19" t="s">
         <v>40</v>
       </c>
-      <c r="G11" s="6"/>
-      <c r="H11" s="6"/>
-      <c r="I11" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="J11" s="6"/>
-      <c r="K11" s="4" t="s">
-        <v>41</v>
-      </c>
     </row>
     <row r="12" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B12" s="7">
+      <c r="B12" s="5">
         <v>1</v>
       </c>
       <c r="C12" t="s">
         <v>4</v>
       </c>
-      <c r="D12" s="8">
-        <v>10</v>
+      <c r="D12" s="6">
+        <v>7</v>
       </c>
       <c r="E12" s="1">
         <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
-      <c r="F12" s="6"/>
-      <c r="G12" s="6"/>
-      <c r="H12" s="6"/>
-      <c r="I12" s="6"/>
-      <c r="J12" s="6"/>
+        <v>7</v>
+      </c>
+      <c r="F12" s="4"/>
+      <c r="G12" s="4"/>
+      <c r="H12" s="4"/>
+      <c r="I12" s="4"/>
+      <c r="J12" s="4"/>
+      <c r="K12" s="19" t="s">
+        <v>64</v>
+      </c>
     </row>
     <row r="13" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B13" s="7">
+      <c r="B13" s="5">
         <v>2</v>
       </c>
       <c r="C13" t="s">
         <v>5</v>
       </c>
-      <c r="D13" s="8">
+      <c r="D13" s="6">
         <v>1</v>
       </c>
       <c r="E13" s="1">
         <f t="shared" si="0"/>
         <v>2</v>
       </c>
-      <c r="F13" s="6"/>
-      <c r="G13" s="6" t="s">
+      <c r="F13" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="G13" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="H13" s="6"/>
-      <c r="I13" s="6"/>
-      <c r="J13" s="6"/>
+      <c r="H13" s="4"/>
+      <c r="I13" s="4"/>
+      <c r="J13" s="4"/>
+      <c r="K13" s="19" t="s">
+        <v>62</v>
+      </c>
     </row>
     <row r="14" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B14" s="7">
+      <c r="B14" s="5">
         <v>6</v>
       </c>
       <c r="C14" t="s">
         <v>23</v>
       </c>
-      <c r="D14" s="8">
+      <c r="D14" s="6">
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="E14" s="1">
         <f t="shared" si="0"/>
         <v>0.42000000000000004</v>
       </c>
-      <c r="F14" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="G14" s="6"/>
-      <c r="H14" s="6"/>
-      <c r="I14" s="6"/>
-      <c r="J14" s="6"/>
-      <c r="K14" s="2"/>
+      <c r="F14" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="G14" s="4"/>
+      <c r="H14" s="4"/>
+      <c r="I14" s="4"/>
+      <c r="J14" s="4"/>
+      <c r="K14" s="23"/>
     </row>
     <row r="15" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B15" s="7">
+      <c r="B15" s="5">
         <v>3</v>
       </c>
       <c r="C15" t="s">
         <v>24</v>
       </c>
-      <c r="D15" s="8">
+      <c r="D15" s="6">
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="E15" s="1">
         <f t="shared" si="0"/>
         <v>0.21000000000000002</v>
       </c>
-      <c r="F15" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="G15" s="6"/>
-      <c r="H15" s="6"/>
-      <c r="I15" s="6"/>
-      <c r="J15" s="6"/>
-      <c r="K15" s="2"/>
+      <c r="F15" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="G15" s="4"/>
+      <c r="H15" s="4"/>
+      <c r="I15" s="4"/>
+      <c r="J15" s="4"/>
+      <c r="K15" s="23"/>
     </row>
     <row r="16" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B16" s="7">
-        <v>1</v>
-      </c>
-      <c r="C16" s="14" t="s">
+      <c r="B16" s="5">
+        <v>1</v>
+      </c>
+      <c r="C16" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="D16" s="8">
+      <c r="D16" s="6">
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="E16" s="1">
         <f t="shared" si="0"/>
         <v>7.0000000000000007E-2</v>
       </c>
-      <c r="F16" s="6"/>
-      <c r="G16" s="6"/>
-      <c r="H16" s="6"/>
-      <c r="I16" s="6"/>
-      <c r="J16" s="6"/>
-      <c r="K16" s="2"/>
+      <c r="F16" s="4"/>
+      <c r="G16" s="4"/>
+      <c r="H16" s="4"/>
+      <c r="I16" s="4"/>
+      <c r="J16" s="4"/>
+      <c r="K16" s="23"/>
     </row>
     <row r="17" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B17" s="7">
+      <c r="B17" s="5">
         <v>2</v>
       </c>
       <c r="C17" t="s">
         <v>25</v>
       </c>
-      <c r="D17" s="8">
+      <c r="D17" s="6">
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="E17" s="1">
         <f t="shared" si="0"/>
         <v>0.14000000000000001</v>
       </c>
-      <c r="F17" s="6"/>
-      <c r="G17" s="6"/>
-      <c r="H17" s="6"/>
-      <c r="I17" s="6"/>
-      <c r="J17" s="6"/>
-      <c r="K17" s="2"/>
+      <c r="F17" s="4"/>
+      <c r="G17" s="4"/>
+      <c r="H17" s="4"/>
+      <c r="I17" s="4"/>
+      <c r="J17" s="4"/>
+      <c r="K17" s="23"/>
     </row>
     <row r="18" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B18" s="7">
+      <c r="B18" s="5">
         <v>1</v>
       </c>
       <c r="C18" t="s">
+        <v>48</v>
+      </c>
+      <c r="D18" s="6">
+        <v>3.85</v>
+      </c>
+      <c r="E18" s="1">
+        <f t="shared" si="0"/>
+        <v>3.85</v>
+      </c>
+      <c r="F18" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="D18" s="8">
-        <v>3.85</v>
-      </c>
-      <c r="E18" s="1">
-        <f t="shared" si="0"/>
-        <v>3.85</v>
-      </c>
-      <c r="F18" s="6" t="s">
+      <c r="G18" s="4"/>
+      <c r="H18" s="4"/>
+      <c r="I18" s="4"/>
+      <c r="J18" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="K18" s="23"/>
+    </row>
+    <row r="19" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B19" s="5">
+        <v>1</v>
+      </c>
+      <c r="C19" t="s">
+        <v>28</v>
+      </c>
+      <c r="D19" s="6">
+        <v>0.8</v>
+      </c>
+      <c r="E19" s="1">
+        <f t="shared" si="0"/>
+        <v>0.8</v>
+      </c>
+      <c r="F19" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="G18" s="6"/>
-      <c r="H18" s="6"/>
-      <c r="I18" s="6"/>
-      <c r="J18" s="6" t="s">
-        <v>63</v>
-      </c>
-      <c r="K18" s="2"/>
-    </row>
-    <row r="19" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B19" s="7">
-        <v>1</v>
-      </c>
-      <c r="C19" t="s">
-        <v>29</v>
-      </c>
-      <c r="D19" s="8">
-        <v>0.8</v>
-      </c>
-      <c r="E19" s="1">
-        <f t="shared" si="0"/>
-        <v>0.8</v>
-      </c>
-      <c r="F19" s="6" t="s">
-        <v>51</v>
-      </c>
-      <c r="G19" s="6"/>
-      <c r="H19" s="6"/>
-      <c r="I19" s="6"/>
-      <c r="J19" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="K19" s="2"/>
+      <c r="G19" s="4"/>
+      <c r="H19" s="4"/>
+      <c r="I19" s="4"/>
+      <c r="J19" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="K19" s="23"/>
     </row>
     <row r="20" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B20" s="7">
+      <c r="B20" s="5">
         <v>1</v>
       </c>
       <c r="C20" t="s">
+        <v>66</v>
+      </c>
+      <c r="D20" s="6">
+        <v>0.1</v>
+      </c>
+      <c r="E20" s="1">
+        <f t="shared" si="0"/>
+        <v>0.1</v>
+      </c>
+      <c r="F20" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="G20" s="4"/>
+      <c r="H20" s="4"/>
+      <c r="I20" s="4"/>
+      <c r="J20" s="4"/>
+      <c r="K20" s="19" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="21" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B21" s="5">
+        <v>1</v>
+      </c>
+      <c r="C21" t="s">
+        <v>67</v>
+      </c>
+      <c r="D21" s="6">
+        <v>0.06</v>
+      </c>
+      <c r="E21" s="1">
+        <f t="shared" si="0"/>
+        <v>0.06</v>
+      </c>
+      <c r="F21" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="G21" s="4"/>
+      <c r="H21" s="4"/>
+      <c r="I21" s="4"/>
+      <c r="J21" s="4"/>
+      <c r="K21" s="19" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="22" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B22" s="5">
+        <v>2</v>
+      </c>
+      <c r="C22" t="s">
+        <v>43</v>
+      </c>
+      <c r="D22" s="6">
+        <v>0.1</v>
+      </c>
+      <c r="E22" s="1">
+        <f t="shared" si="0"/>
+        <v>0.2</v>
+      </c>
+      <c r="F22" s="4"/>
+      <c r="G22" s="4"/>
+      <c r="H22" s="4"/>
+      <c r="I22" s="4"/>
+      <c r="J22" s="4"/>
+      <c r="K22" s="22"/>
+    </row>
+    <row r="23" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B23" s="5">
+        <v>1</v>
+      </c>
+      <c r="C23" t="s">
+        <v>59</v>
+      </c>
+      <c r="D23" s="6">
+        <v>0.2</v>
+      </c>
+      <c r="E23" s="1">
+        <f t="shared" si="0"/>
+        <v>0.2</v>
+      </c>
+      <c r="F23" s="4"/>
+      <c r="G23" s="4"/>
+      <c r="H23" s="4"/>
+      <c r="I23" s="4"/>
+      <c r="J23" s="4"/>
+      <c r="K23" s="22"/>
+    </row>
+    <row r="24" spans="2:11" x14ac:dyDescent="0.25">
+      <c r="B24" s="5"/>
+      <c r="C24" t="s">
         <v>53</v>
       </c>
-      <c r="D20" s="8">
-        <v>0.1</v>
-      </c>
-      <c r="E20" s="1">
-        <f t="shared" si="0"/>
-        <v>0.1</v>
-      </c>
-      <c r="F20" s="6"/>
-      <c r="G20" s="6"/>
-      <c r="H20" s="6"/>
-      <c r="I20" s="6"/>
-      <c r="J20" s="6"/>
-    </row>
-    <row r="21" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B21" s="7">
-        <v>1</v>
-      </c>
-      <c r="C21" t="s">
-        <v>28</v>
-      </c>
-      <c r="D21" s="8">
-        <v>0.1</v>
-      </c>
-      <c r="E21" s="1">
-        <f t="shared" si="0"/>
-        <v>0.1</v>
-      </c>
-      <c r="F21" s="6"/>
-      <c r="G21" s="6"/>
-      <c r="H21" s="6"/>
-      <c r="I21" s="6"/>
-      <c r="J21" s="6"/>
-    </row>
-    <row r="22" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B22" s="7">
-        <v>2</v>
-      </c>
-      <c r="C22" t="s">
-        <v>44</v>
-      </c>
-      <c r="D22" s="8">
-        <v>0.1</v>
-      </c>
-      <c r="E22" s="1">
-        <f t="shared" si="0"/>
-        <v>0.2</v>
-      </c>
-      <c r="F22" s="6"/>
-      <c r="G22" s="6"/>
-      <c r="H22" s="6"/>
-      <c r="I22" s="6"/>
-      <c r="J22" s="6"/>
-    </row>
-    <row r="23" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B23" s="7">
-        <v>1</v>
-      </c>
-      <c r="C23" t="s">
-        <v>61</v>
-      </c>
-      <c r="D23" s="8">
-        <v>0.2</v>
-      </c>
-      <c r="E23" s="1">
-        <f t="shared" si="0"/>
-        <v>0.2</v>
-      </c>
-      <c r="F23" s="6"/>
-      <c r="G23" s="6"/>
-      <c r="H23" s="6"/>
-      <c r="I23" s="6"/>
-      <c r="J23" s="6"/>
-    </row>
-    <row r="24" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="B24" s="7"/>
-      <c r="C24" t="s">
-        <v>55</v>
-      </c>
-      <c r="D24" s="8">
+      <c r="D24" s="6">
         <v>1.9</v>
       </c>
       <c r="E24" s="1">
         <f>D25*B24</f>
         <v>0</v>
       </c>
-      <c r="F24" s="6" t="s">
-        <v>59</v>
-      </c>
-      <c r="G24" s="6"/>
-      <c r="H24" s="6"/>
-      <c r="I24" s="6" t="s">
+      <c r="F24" s="4" t="s">
         <v>57</v>
       </c>
-      <c r="J24" s="6"/>
-      <c r="K24" s="4" t="s">
-        <v>58</v>
+      <c r="G24" s="4"/>
+      <c r="H24" s="4"/>
+      <c r="I24" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="J24" s="4"/>
+      <c r="K24" s="19" t="s">
+        <v>56</v>
       </c>
     </row>
     <row r="25" spans="2:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B25" s="10"/>
-      <c r="C25" s="11" t="s">
-        <v>54</v>
-      </c>
-      <c r="D25" s="12">
+      <c r="B25" s="8"/>
+      <c r="C25" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="D25" s="10">
         <v>13.46</v>
       </c>
-      <c r="E25" s="13">
+      <c r="E25" s="11">
         <f>D26*B25</f>
         <v>0</v>
       </c>
-      <c r="F25" s="17"/>
-      <c r="G25" s="17"/>
-      <c r="H25" s="17"/>
-      <c r="I25" s="17" t="s">
-        <v>56</v>
-      </c>
-      <c r="J25" s="17"/>
-      <c r="K25" s="11"/>
+      <c r="F25" s="15"/>
+      <c r="G25" s="15"/>
+      <c r="H25" s="15"/>
+      <c r="I25" s="15" t="s">
+        <v>54</v>
+      </c>
+      <c r="J25" s="15"/>
+      <c r="K25" s="9"/>
     </row>
     <row r="26" spans="2:11" x14ac:dyDescent="0.25">
       <c r="E26" s="1">
         <f>SUM(E4:E25)</f>
-        <v>77.879999999999967</v>
+        <v>74.839999999999975</v>
       </c>
     </row>
     <row r="27" spans="2:11" x14ac:dyDescent="0.25">
@@ -1264,27 +1330,27 @@
       </c>
     </row>
     <row r="28" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="C28" s="5" t="s">
+      <c r="C28" s="3" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="29" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="C29" s="5" t="s">
+      <c r="C29" s="3" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="30" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="C30" s="5" t="s">
+      <c r="C30" s="3" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="31" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="C31" s="5" t="s">
+      <c r="C31" s="3" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="32" spans="2:11" x14ac:dyDescent="0.25">
-      <c r="C32" s="5" t="s">
+      <c r="C32" s="3" t="s">
         <v>27</v>
       </c>
     </row>

</xml_diff>